<commit_message>
Requested fixes for 1.1.0
</commit_message>
<xml_diff>
--- a/data-raw/input/musicassessr_dict_sabeth_neue_version.xlsx
+++ b/data-raw/input/musicassessr_dict_sabeth_neue_version.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/singpause/data-raw/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebsilas/songbird/data-raw/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA10524-4258-0149-BACF-D2F93D98745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434C9CF1-56F0-6446-BCE4-A2254449313D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="3" xr2:uid="{551E65E8-47F0-CE49-A457-DBD11DAE7EF5}"/>
   </bookViews>
@@ -20,6 +20,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$D$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tabelle3!$A$1:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Tabelle4!$A$1:$D$181</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1651" uniqueCount="984">
   <si>
     <t>mar_can_hear</t>
   </si>
@@ -3017,6 +3019,12 @@
   </si>
   <si>
     <t>Mochtest du weiterlernen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danke! Du hast das </t>
+  </si>
+  <si>
+    <t>Toll gemacht!</t>
   </si>
 </sst>
 </file>
@@ -3512,8 +3520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A169A32C-6679-F443-A7A2-ABDC5FD4F6B4}">
   <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView topLeftCell="C59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D164"/>
+    <sheetView topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6529,7 +6537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A22DF3B7-8878-064B-9246-F0834514B2BF}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6754,6 +6764,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C13" xr:uid="{A22DF3B7-8878-064B-9246-F0834514B2BF}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6762,8 +6773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19D2AA2-7F7B-C743-8F66-202935957A13}">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A181" sqref="A181"/>
+    <sheetView tabSelected="1" topLeftCell="C155" zoomScale="115" workbookViewId="0">
+      <selection activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7776,7 +7787,7 @@
         <v>110</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>261</v>
+        <v>982</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>859</v>
@@ -9135,7 +9146,7 @@
         <v>944</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>945</v>
+        <v>983</v>
       </c>
       <c r="D169" s="12" t="s">
         <v>945</v>
@@ -9315,6 +9326,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D181" xr:uid="{A19D2AA2-7F7B-C743-8F66-202935957A13}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>